<commit_message>
refactor code for derived values
</commit_message>
<xml_diff>
--- a/input/data_1-raw/RXF Fuels Data for R 2022-02-07.xlsx
+++ b/input/data_1-raw/RXF Fuels Data for R 2022-02-07.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgray/Documents/GitHub/woody-fuels/input/raw-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgray/Documents/GitHub/woody-fuels/input/data_1-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46AEC51-6829-664D-AE06-C93E9E501104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B843AC1-8FF5-8349-BBDC-9E9C966BA59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24240" windowHeight="19580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24240" windowHeight="19580" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="55" r:id="rId1"/>
@@ -842,7 +842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A8973D-263C-4A46-915C-3903CB9E3DE2}">
   <dimension ref="A1:H433"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F1" sqref="A1:XFD1048576"/>
     </sheetView>
@@ -11498,8 +11498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53BCC2AB-A162-464C-9CA8-0C738B0B1B2C}">
   <dimension ref="A1:C16385"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>